<commit_message>
Add and update sprint file and ppt.
Add and update this week's objectives in the sprint file and workshop 1 ppt.
</commit_message>
<xml_diff>
--- a/Project_Files/GDP-02-Sprint04/Stand-up Meeting Sec03Team05 Sprint04.xlsx
+++ b/Project_Files/GDP-02-Sprint04/Stand-up Meeting Sec03Team05 Sprint04.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Desktop\FreebiesforNewbies\Project_Files\GDP-02-Sprint04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/FreebiesforNewbies/Project_Files/GDP-02-Sprint04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68B3500-7DE8-4DF3-8A78-3F4B42F58D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{F68B3500-7DE8-4DF3-8A78-3F4B42F58D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71EF324F-C7C7-47CD-9F23-9C9D7BECDB41}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Daily Stand-up Meeting Report</t>
   </si>
@@ -159,6 +159,24 @@
   </si>
   <si>
     <t>We are stuck in these functionalities and planning to complete</t>
+  </si>
+  <si>
+    <t>created and done changes in the event delete detail page</t>
+  </si>
+  <si>
+    <t>Creating slides for workshop</t>
+  </si>
+  <si>
+    <t>Created slides for the workshop</t>
+  </si>
+  <si>
+    <t>Planning new layouts for the free event page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planned new layouts for the free events </t>
+  </si>
+  <si>
+    <t>Creating activities like create activities for free activity.</t>
   </si>
 </sst>
 </file>
@@ -763,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1264,9 +1282,15 @@
       <c r="A17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1292,9 +1316,15 @@
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1">
       <c r="A18" s="10"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1320,9 +1350,15 @@
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1">
       <c r="A19" s="11"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>

</xml_diff>